<commit_message>
Coulombparameter für die Stäbe hinzugefügt
</commit_message>
<xml_diff>
--- a/Modellparameter/ParameterHistorie.xlsx
+++ b/Modellparameter/ParameterHistorie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Frederik Tesar\Documents\_Studium\12. Semester\Projektseminar Regelungstechnik\PS 2020 Doppelpendel Simulation\Modellparameter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B9AD03-88C7-4CE4-849A-42A7D34CF5AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081C324C-8911-4E92-BF34-E0128A50F418}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{E0B92372-9177-4C06-8BF1-F3E1AFEF8F80}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E0B92372-9177-4C06-8BF1-F3E1AFEF8F80}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -697,13 +697,13 @@
     <t>Größe</t>
   </si>
   <si>
-    <t>Spalte1</t>
-  </si>
-  <si>
-    <t>Spalte2</t>
-  </si>
-  <si>
-    <t>Spalte3</t>
+    <t>Kisner112</t>
+  </si>
+  <si>
+    <t>Chang192</t>
+  </si>
+  <si>
+    <t>Ribeiro202</t>
   </si>
 </sst>
 </file>
@@ -808,12 +808,12 @@
     <tableColumn id="7" xr3:uid="{652A53E2-8F42-425C-AEFD-4DC77CD7D3D4}" name="Kämmerer09"/>
     <tableColumn id="8" xr3:uid="{BBF57FF6-44F0-454F-9913-526296225CD4}" name="Noupa11"/>
     <tableColumn id="9" xr3:uid="{7F54FF13-6D7B-4014-87BE-4ACB61A23F70}" name="Kisner11"/>
-    <tableColumn id="10" xr3:uid="{539BF4C4-A9BB-4059-B11E-84DE03F2AE44}" name="Spalte1"/>
+    <tableColumn id="10" xr3:uid="{539BF4C4-A9BB-4059-B11E-84DE03F2AE44}" name="Kisner112"/>
     <tableColumn id="11" xr3:uid="{24B15311-BCBD-4369-9B7E-9E48815BC94B}" name="Brehl14"/>
     <tableColumn id="12" xr3:uid="{4F4F0447-D771-41E5-A61C-7BAF382A919C}" name="Chang19"/>
-    <tableColumn id="13" xr3:uid="{9F7BF82E-678E-46DA-9889-1672EB77E061}" name="Spalte2"/>
+    <tableColumn id="13" xr3:uid="{9F7BF82E-678E-46DA-9889-1672EB77E061}" name="Chang192"/>
     <tableColumn id="14" xr3:uid="{54F32CDC-043F-457D-B089-CECF5751A955}" name="Ribeiro20"/>
-    <tableColumn id="15" xr3:uid="{B09F39A7-980F-4D6F-9FDE-E0F86CBA3987}" name="Spalte3"/>
+    <tableColumn id="15" xr3:uid="{B09F39A7-980F-4D6F-9FDE-E0F86CBA3987}" name="Ribeiro202"/>
     <tableColumn id="16" xr3:uid="{1946E82A-9434-45D1-B3DC-DB6C92E61F3D}" name="Fauvé20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1209,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50455A25-6E7D-4307-9996-8B486D0CEF10}">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Korrektur Parameterhistorie.xlsx J2 Ribeiro20 + allg Anpassungen
</commit_message>
<xml_diff>
--- a/Modellparameter/ParameterHistorie.xlsx
+++ b/Modellparameter/ParameterHistorie.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Frederik Tesar\Documents\_Studium\12. Semester\Projektseminar Regelungstechnik\PS 2020 Doppelpendel Simulation\Modellparameter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081C324C-8911-4E92-BF34-E0128A50F418}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C5AB08-965B-4BC8-8B33-CC54F1083552}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E0B92372-9177-4C06-8BF1-F3E1AFEF8F80}"/>
   </bookViews>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1209,8 +1211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50455A25-6E7D-4307-9996-8B486D0CEF10}">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1536,7 +1538,7 @@
         <v>3.3400000000000001E-3</v>
       </c>
       <c r="N12" s="8">
-        <v>3.4299999999999999E-3</v>
+        <v>3.3430000000000001E-3</v>
       </c>
       <c r="O12" s="8">
         <v>3.0000000000000001E-3</v>

</xml_diff>